<commit_message>
add final clinical challenge study data
all final clinical challenge material
</commit_message>
<xml_diff>
--- a/clinical-challenge-study-data.xlsx
+++ b/clinical-challenge-study-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tavis.anderson/Desktop/local-repos/dairy-cattle-hpai-experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usdagcc-my.sharepoint.com/personal/amy_l_baker_usda_gov/Documents/HPAI cattle experiment manuscript/Nature revision/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CE9D5D5-73A4-5743-B37F-2910C61CDD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="14_{702E48F3-56C5-C94F-BBFF-E6B3B779F305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5974E930-28C5-7D45-AE53-C8B2DF8DFAAC}"/>
   <bookViews>
-    <workbookView xWindow="35000" yWindow="500" windowWidth="44120" windowHeight="25860" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34960" yWindow="500" windowWidth="29780" windowHeight="26380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Milk Scoring" sheetId="4" r:id="rId1"/>
@@ -1249,7 +1249,7 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:L25"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12746,8 +12746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E1FD94-D165-43AB-8616-BBED31380E0F}">
   <dimension ref="A1:G486"/>
   <sheetViews>
-    <sheetView topLeftCell="A340" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26393,8 +26393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F15C018-A361-421C-AAB2-1D20D4F8193E}">
   <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>